<commit_message>
beefban greedy and russia march greedy tests
</commit_message>
<xml_diff>
--- a/tests_greedy/beefban_greedy_complete_graphs.xlsx
+++ b/tests_greedy/beefban_greedy_complete_graphs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>deltaRwc (in deg)</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>RWC Descent (ratio)</t>
+  </si>
+  <si>
+    <t>RWC Opt Descent (in deg)</t>
+  </si>
+  <si>
+    <t>RWC Opt Descent (ratio)</t>
   </si>
 </sst>
 </file>
@@ -237,7 +243,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$K$2:$K$21</c:f>
+              <c:f>Foglio1!$L$2:$L$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -316,11 +322,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="138113408"/>
-        <c:axId val="138114944"/>
+        <c:axId val="227116160"/>
+        <c:axId val="227118080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="138113408"/>
+        <c:axId val="227116160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -348,7 +354,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138114944"/>
+        <c:crossAx val="227118080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -356,7 +362,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="138114944"/>
+        <c:axId val="227118080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -391,7 +397,308 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138113408"/>
+        <c:crossAx val="227116160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT"/>
+              <a:t>Optimum RWC Descent</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>RWC Descent (in deg)</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$G$2:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.8555252931950741</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8544817938824385</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8043325606007126</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7589073157427855</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.731631820218245</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7163339775346746</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7021002347425518</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6896564579730979</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6777384134615598</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.666401464821283</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.6631826275287123</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.662073728502961</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.6615862022887964</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.6503733239989935</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.6394183758091272</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.6267878835669238</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6160943217217667</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.6070328158064744</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.5988479273358163</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.590644444167673</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>RWC Descent (ratio)</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$M$2:$M$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.8807353713533519</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.839227867801519</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8010220689576864</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7644508855275673</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7183685827489374</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6889591812937708</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6722581880801386</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6556717541955075</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6396662362655698</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.6250564318582306</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.6105273077216913</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.5976636698164606</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.5852275565615175</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.5733255596636877</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.5614513477494221</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5502065428614598</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.5391383703929378</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.5284102074407708</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.5177628269216334</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.5071621697840321</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="149698432"/>
+        <c:axId val="153641728"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="149698432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>edge</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="153641728"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="153641728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>rwc score</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="149698432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -440,6 +747,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1085850</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Grafico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -735,10 +1072,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,13 +1085,16 @@
     <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -770,20 +1110,26 @@
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.98924722</v>
       </c>
@@ -801,22 +1147,30 @@
         <f xml:space="preserve"> $A$2 + E2</f>
         <v>1.9891458130787627</v>
       </c>
-      <c r="H2">
+      <c r="G2">
+        <f xml:space="preserve"> $A$2 + C2</f>
+        <v>1.8555252931950741</v>
+      </c>
+      <c r="I2">
         <v>-0.10851184864664799</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>7.5834175935288097E-4</v>
       </c>
-      <c r="J2">
-        <f>H2*I2</f>
+      <c r="K2">
+        <f>I2*J2</f>
         <v>-8.2289066213332571E-5</v>
       </c>
-      <c r="K2">
-        <f>$A$2 + J2</f>
+      <c r="L2">
+        <f>$A$2 + K2</f>
         <v>1.9891649309337867</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <f>$A$2+I2</f>
+        <v>1.8807353713533519</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>-1.0434993126356099E-3</v>
       </c>
@@ -831,22 +1185,30 @@
         <f xml:space="preserve"> F2 + E3</f>
         <v>1.98910059433581</v>
       </c>
-      <c r="H3">
+      <c r="G3">
+        <f xml:space="preserve"> G2+C3</f>
+        <v>1.8544817938824385</v>
+      </c>
+      <c r="I3">
         <v>-4.15075035518329E-2</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>8.3375442142496201E-4</v>
       </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J21" si="1">H3*I3</f>
+      <c r="K3">
+        <f t="shared" ref="K3:K21" si="1">I3*J3</f>
         <v>-3.4607064608652998E-5</v>
       </c>
-      <c r="K3">
-        <f>K2 + J3</f>
+      <c r="L3">
+        <f>L2 + K3</f>
         <v>1.989130323869178</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <f>M2+I3</f>
+        <v>1.839227867801519</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>-5.0149233281725998E-2</v>
       </c>
@@ -861,22 +1223,30 @@
         <f t="shared" ref="F4:F21" si="2" xml:space="preserve"> F3 + E4</f>
         <v>1.9890550041237356</v>
       </c>
-      <c r="H4">
+      <c r="G4">
+        <f t="shared" ref="G4:G21" si="3" xml:space="preserve"> G3+C4</f>
+        <v>1.8043325606007126</v>
+      </c>
+      <c r="I4">
         <v>-3.82057988438326E-2</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>9.0909090909090898E-4</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <f t="shared" si="1"/>
         <v>-3.4732544403484179E-5</v>
       </c>
-      <c r="K4">
-        <f t="shared" ref="K4:K21" si="3">K3 + J4</f>
+      <c r="L4">
+        <f t="shared" ref="L4:L21" si="4">L3 + K4</f>
         <v>1.9890955913247745</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <f t="shared" ref="M4:M21" si="5">M3+I4</f>
+        <v>1.8010220689576864</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>-4.5425244857927198E-2</v>
       </c>
@@ -891,22 +1261,30 @@
         <f t="shared" si="2"/>
         <v>1.989010289723194</v>
       </c>
-      <c r="H5">
+      <c r="G5">
+        <f t="shared" si="3"/>
+        <v>1.7589073157427855</v>
+      </c>
+      <c r="I5">
         <v>-3.6571183430118899E-2</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>9.8435133770822798E-4</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <f t="shared" si="1"/>
         <v>-3.5998893331010521E-5</v>
       </c>
-      <c r="K5">
-        <f t="shared" si="3"/>
+      <c r="L5">
+        <f t="shared" si="4"/>
         <v>1.9890595924314436</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <f t="shared" si="5"/>
+        <v>1.7644508855275673</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>-2.7275495524540401E-2</v>
       </c>
@@ -921,22 +1299,30 @@
         <f t="shared" si="2"/>
         <v>1.988981390358612</v>
       </c>
-      <c r="H6">
+      <c r="G6">
+        <f t="shared" si="3"/>
+        <v>1.731631820218245</v>
+      </c>
+      <c r="I6">
         <v>-4.6082302778629902E-2</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>1.05953582240161E-3</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <f t="shared" si="1"/>
         <v>-4.8825850572715635E-5</v>
       </c>
-      <c r="K6">
-        <f t="shared" si="3"/>
+      <c r="L6">
+        <f t="shared" si="4"/>
         <v>1.9890107665808709</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <f t="shared" si="5"/>
+        <v>1.7183685827489374</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>-1.5297842683570401E-2</v>
       </c>
@@ -951,22 +1337,30 @@
         <f t="shared" si="2"/>
         <v>1.9889640327458848</v>
       </c>
-      <c r="H7">
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>1.7163339775346746</v>
+      </c>
+      <c r="I7">
         <v>-2.9409401455166601E-2</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>1.1346444780635399E-3</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <f t="shared" si="1"/>
         <v>-3.3369214964258618E-5</v>
       </c>
-      <c r="K7">
-        <f t="shared" si="3"/>
+      <c r="L7">
+        <f t="shared" si="4"/>
         <v>1.9889773973659066</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <f t="shared" si="5"/>
+        <v>1.6889591812937708</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>-1.4233742792122899E-2</v>
       </c>
@@ -981,22 +1375,30 @@
         <f t="shared" si="2"/>
         <v>1.9889468145086364</v>
       </c>
-      <c r="H8">
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>1.7021002347425518</v>
+      </c>
+      <c r="I8">
         <v>-1.67009932136322E-2</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>1.2096774193548301E-3</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <f t="shared" si="1"/>
         <v>-2.0202814371329131E-5</v>
       </c>
-      <c r="K8">
-        <f t="shared" si="3"/>
+      <c r="L8">
+        <f t="shared" si="4"/>
         <v>1.9889571945515352</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <f t="shared" si="5"/>
+        <v>1.6722581880801386</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>-1.24437767694539E-2</v>
       </c>
@@ -1011,22 +1413,30 @@
         <f t="shared" si="2"/>
         <v>1.9889308288004439</v>
       </c>
-      <c r="H9">
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>1.6896564579730979</v>
+      </c>
+      <c r="I9">
         <v>-1.6586433884631099E-2</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>1.28463476070529E-3</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <f t="shared" si="1"/>
         <v>-2.1307509524337186E-5</v>
       </c>
-      <c r="K9">
-        <f t="shared" si="3"/>
+      <c r="L9">
+        <f t="shared" si="4"/>
         <v>1.9889358870420109</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <f t="shared" si="5"/>
+        <v>1.6556717541955075</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>-1.19180445115382E-2</v>
       </c>
@@ -1041,22 +1451,30 @@
         <f t="shared" si="2"/>
         <v>1.9889146260208965</v>
       </c>
-      <c r="H10">
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>1.6777384134615598</v>
+      </c>
+      <c r="I10">
         <v>-1.60055179299376E-2</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>1.3595166163141901E-3</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <f t="shared" si="1"/>
         <v>-2.1759767578464866E-5</v>
       </c>
-      <c r="K10">
-        <f t="shared" si="3"/>
+      <c r="L10">
+        <f t="shared" si="4"/>
         <v>1.9889141272744324</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <f t="shared" si="5"/>
+        <v>1.6396662362655698</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>-1.13369486402768E-2</v>
       </c>
@@ -1071,22 +1489,30 @@
         <f t="shared" si="2"/>
         <v>1.9888983651735765</v>
       </c>
-      <c r="H11">
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>1.666401464821283</v>
+      </c>
+      <c r="I11">
         <v>-1.46098044073393E-2</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>1.4343231001509799E-3</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <f t="shared" si="1"/>
         <v>-2.0955179950134355E-5</v>
       </c>
-      <c r="K11">
-        <f t="shared" si="3"/>
+      <c r="L11">
+        <f t="shared" si="4"/>
         <v>1.9888931720944822</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <f t="shared" si="5"/>
+        <v>1.6250564318582306</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>-3.2188372925706999E-3</v>
       </c>
@@ -1101,22 +1527,30 @@
         <f t="shared" si="2"/>
         <v>1.9887567071883014</v>
       </c>
-      <c r="H12">
+      <c r="G12">
+        <f t="shared" si="3"/>
+        <v>1.6631826275287123</v>
+      </c>
+      <c r="I12">
         <v>-1.4529124136539199E-2</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>1.50905432595573E-3</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <f t="shared" si="1"/>
         <v>-2.1925237630592288E-5</v>
       </c>
-      <c r="K12">
-        <f t="shared" si="3"/>
+      <c r="L12">
+        <f t="shared" si="4"/>
         <v>1.9888712468568517</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <f t="shared" si="5"/>
+        <v>1.6105273077216913</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>-1.1088990257513899E-3</v>
       </c>
@@ -1131,22 +1565,30 @@
         <f t="shared" si="2"/>
         <v>1.9887078228047794</v>
       </c>
-      <c r="H13">
+      <c r="G13">
+        <f t="shared" si="3"/>
+        <v>1.662073728502961</v>
+      </c>
+      <c r="I13">
         <v>-1.2863637905230801E-2</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>1.5837104072398099E-3</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <f t="shared" si="1"/>
         <v>-2.0372277225478526E-5</v>
       </c>
-      <c r="K13">
-        <f t="shared" si="3"/>
+      <c r="L13">
+        <f t="shared" si="4"/>
         <v>1.9888508745796263</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <f t="shared" si="5"/>
+        <v>1.5976636698164606</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>-4.8752621416459899E-4</v>
       </c>
@@ -1161,22 +1603,30 @@
         <f t="shared" si="2"/>
         <v>1.9886862944801214</v>
       </c>
-      <c r="H14">
+      <c r="G14">
+        <f t="shared" si="3"/>
+        <v>1.6615862022887964</v>
+      </c>
+      <c r="I14">
         <v>-1.2436113254942999E-2</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>1.65829145728643E-3</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <f t="shared" si="1"/>
         <v>-2.0622700372518515E-5</v>
       </c>
-      <c r="K14">
-        <f t="shared" si="3"/>
+      <c r="L14">
+        <f t="shared" si="4"/>
         <v>1.9888302518792538</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <f t="shared" si="5"/>
+        <v>1.5852275565615175</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>-1.1212878289802899E-2</v>
       </c>
@@ -1191,22 +1641,30 @@
         <f t="shared" si="2"/>
         <v>1.9886668648316534</v>
       </c>
-      <c r="H15">
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>1.6503733239989935</v>
+      </c>
+      <c r="I15">
         <v>-1.1901996897829699E-2</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>1.73279758915118E-3</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <f t="shared" si="1"/>
         <v>-2.0623751530644125E-5</v>
       </c>
-      <c r="K15">
-        <f t="shared" si="3"/>
+      <c r="L15">
+        <f t="shared" si="4"/>
         <v>1.9888096281277232</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <f t="shared" si="5"/>
+        <v>1.5733255596636877</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>-1.0954948189866399E-2</v>
       </c>
@@ -1221,22 +1679,30 @@
         <f t="shared" si="2"/>
         <v>1.9886470667325151</v>
       </c>
-      <c r="H16">
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>1.6394183758091272</v>
+      </c>
+      <c r="I16">
         <v>-1.18742119142656E-2</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>1.80722891566265E-3</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <f t="shared" si="1"/>
         <v>-2.1459419122166741E-5</v>
       </c>
-      <c r="K16">
-        <f t="shared" si="3"/>
+      <c r="L16">
+        <f t="shared" si="4"/>
         <v>1.9887881687086011</v>
       </c>
-    </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <f t="shared" si="5"/>
+        <v>1.5614513477494221</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>-1.26304922422034E-2</v>
       </c>
@@ -1251,22 +1717,30 @@
         <f t="shared" si="2"/>
         <v>1.9886233013808301</v>
       </c>
-      <c r="H17">
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>1.6267878835669238</v>
+      </c>
+      <c r="I17">
         <v>-1.12448048879623E-2</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>1.8815855494229801E-3</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <f t="shared" si="1"/>
         <v>-2.1158062383270756E-5</v>
       </c>
-      <c r="K17">
-        <f t="shared" si="3"/>
+      <c r="L17">
+        <f t="shared" si="4"/>
         <v>1.9887670106462179</v>
       </c>
-    </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <f t="shared" si="5"/>
+        <v>1.5502065428614598</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>-1.06935618451571E-2</v>
       </c>
@@ -1281,22 +1755,30 @@
         <f t="shared" si="2"/>
         <v>1.9886023861896585</v>
       </c>
-      <c r="H18">
+      <c r="G18">
+        <f t="shared" si="3"/>
+        <v>1.6160943217217667</v>
+      </c>
+      <c r="I18">
         <v>-1.1068172468521899E-2</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>1.95586760280842E-3</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <f t="shared" si="1"/>
         <v>-2.1647879953478079E-5</v>
       </c>
-      <c r="K18">
-        <f t="shared" si="3"/>
+      <c r="L18">
+        <f t="shared" si="4"/>
         <v>1.9887453627662643</v>
       </c>
-    </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <f t="shared" si="5"/>
+        <v>1.5391383703929378</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>-9.0615059152924001E-3</v>
       </c>
@@ -1311,22 +1793,30 @@
         <f t="shared" si="2"/>
         <v>1.9885839906513343</v>
       </c>
-      <c r="H19">
+      <c r="G19">
+        <f t="shared" si="3"/>
+        <v>1.6070328158064744</v>
+      </c>
+      <c r="I19">
         <v>-1.07281629521669E-2</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>2.0300751879699201E-3</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <f t="shared" si="1"/>
         <v>-2.1778977421692154E-5</v>
       </c>
-      <c r="K19">
-        <f t="shared" si="3"/>
+      <c r="L19">
+        <f t="shared" si="4"/>
         <v>1.9887235837888426</v>
       </c>
-    </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <f t="shared" si="5"/>
+        <v>1.5284102074407708</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>-8.1848884706580902E-3</v>
       </c>
@@ -1341,22 +1831,30 @@
         <f t="shared" si="2"/>
         <v>1.9885667679401235</v>
       </c>
-      <c r="H20">
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>1.5988479273358163</v>
+      </c>
+      <c r="I20">
         <v>-1.0647380519137301E-2</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>4.4604208416833602E-2</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <f t="shared" si="1"/>
         <v>-4.7491797976893411E-4</v>
       </c>
-      <c r="K20">
-        <f t="shared" si="3"/>
+      <c r="L20">
+        <f t="shared" si="4"/>
         <v>1.9882486658090737</v>
       </c>
-    </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <f t="shared" si="5"/>
+        <v>1.5177628269216334</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>-8.2034831681432503E-3</v>
       </c>
@@ -1371,19 +1869,27 @@
         <f t="shared" si="2"/>
         <v>1.9885488985601629</v>
       </c>
-      <c r="H21">
+      <c r="G21">
+        <f t="shared" si="3"/>
+        <v>1.590644444167673</v>
+      </c>
+      <c r="I21">
         <v>-1.06006571376014E-2</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>2.1782674011016499E-3</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <f t="shared" si="1"/>
         <v>-2.3091065873092659E-5</v>
       </c>
-      <c r="K21">
-        <f t="shared" si="3"/>
+      <c r="L21">
+        <f t="shared" si="4"/>
         <v>1.9882255747432005</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="5"/>
+        <v>1.5071621697840321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
indiana greedy complete graphs
</commit_message>
<xml_diff>
--- a/tests_greedy/beefban_greedy_complete_graphs.xlsx
+++ b/tests_greedy/beefban_greedy_complete_graphs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>deltaRwc (in deg)</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>RWC Opt Descent (ratio)</t>
+  </si>
+  <si>
+    <t>inter-community edges ratio</t>
   </si>
 </sst>
 </file>
@@ -322,11 +325,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="227116160"/>
-        <c:axId val="227118080"/>
+        <c:axId val="272664448"/>
+        <c:axId val="272670720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="227116160"/>
+        <c:axId val="272664448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -354,7 +357,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="227118080"/>
+        <c:crossAx val="272670720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -362,7 +365,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="227118080"/>
+        <c:axId val="272670720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -397,7 +400,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="227116160"/>
+        <c:crossAx val="272664448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -628,11 +631,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="149698432"/>
-        <c:axId val="153641728"/>
+        <c:axId val="273036800"/>
+        <c:axId val="273038720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="149698432"/>
+        <c:axId val="273036800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -660,7 +663,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153641728"/>
+        <c:crossAx val="273038720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -668,7 +671,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153641728"/>
+        <c:axId val="273038720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -698,7 +701,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149698432"/>
+        <c:crossAx val="273036800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1072,10 +1075,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1702,7 +1705,7 @@
         <v>1.5614513477494221</v>
       </c>
     </row>
-    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>-1.26304922422034E-2</v>
       </c>
@@ -1740,7 +1743,7 @@
         <v>1.5502065428614598</v>
       </c>
     </row>
-    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>-1.06935618451571E-2</v>
       </c>
@@ -1778,7 +1781,7 @@
         <v>1.5391383703929378</v>
       </c>
     </row>
-    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>-9.0615059152924001E-3</v>
       </c>
@@ -1816,7 +1819,7 @@
         <v>1.5284102074407708</v>
       </c>
     </row>
-    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>-8.1848884706580902E-3</v>
       </c>
@@ -1854,7 +1857,7 @@
         <v>1.5177628269216334</v>
       </c>
     </row>
-    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>-8.2034831681432503E-3</v>
       </c>
@@ -1890,6 +1893,16 @@
       <c r="M21">
         <f t="shared" si="5"/>
         <v>1.5071621697840321</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>5.5579999999999996E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>